<commit_message>
Fixture Standard, TRL and SOLT calibration kit done
</commit_message>
<xml_diff>
--- a/V1I1/! Docs/MW101-TRLCalc-rev1.xlsx
+++ b/V1I1/! Docs/MW101-TRLCalc-rev1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\SiP Sigfox\Hardware\Work\designFlow_RFmodeling\V1I1\! Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743EFBD2-5242-4AC4-BDBB-C9E01D6D7AC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B624D6-41DA-4132-9C81-61A89471F279}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11626,8 +11626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A4:AQ118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>